<commit_message>
test configs created from tuned configs
</commit_message>
<xml_diff>
--- a/Configurations.xlsx
+++ b/Configurations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cce1d1199b24a628/Code/DE Assignments/Configuration YAMLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{8D0E1276-EBAA-4732-837E-8ED9B2BF1DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD617B2F-5862-423F-B934-1FE7A91E4FBD}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="8_{8D0E1276-EBAA-4732-837E-8ED9B2BF1DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DFBB65E6-550E-4732-9DDA-97D560E6B1F4}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="21">
   <si>
     <t>Entry No.</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>Time terminated</t>
+  </si>
+  <si>
+    <t>50, 100, 150</t>
+  </si>
+  <si>
+    <t>Total time</t>
   </si>
 </sst>
 </file>
@@ -641,7 +647,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -669,14 +675,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -687,8 +690,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1045,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AO23"/>
+  <dimension ref="A1:AP23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AO2" sqref="AO2"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,75 +1067,76 @@
     <col min="3" max="9" width="9.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="9.5703125" style="1" customWidth="1"/>
     <col min="11" max="11" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="40" width="9.140625" style="1"/>
-    <col min="41" max="41" width="150" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="41" width="9.140625" style="1"/>
+    <col min="42" max="42" width="150" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="15" t="s">
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15" t="s">
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15" t="s">
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15" t="s">
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
+      <c r="Y1" s="20"/>
+      <c r="Z1" s="20"/>
+      <c r="AA1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="20" t="s">
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="AG1" s="20"/>
-      <c r="AH1" s="20"/>
-      <c r="AI1" s="20"/>
-      <c r="AJ1" s="20"/>
-      <c r="AK1" s="15" t="s">
+      <c r="AG1" s="19"/>
+      <c r="AH1" s="19"/>
+      <c r="AI1" s="19"/>
+      <c r="AJ1" s="19"/>
+      <c r="AK1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="16" t="s">
+      <c r="AL1" s="20"/>
+      <c r="AM1" s="15"/>
+      <c r="AN1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AN1" s="17"/>
+      <c r="AO1" s="22"/>
     </row>
-    <row r="2" spans="1:41" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19"/>
+    <row r="2" spans="1:42" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
@@ -1239,14 +1249,17 @@
         <v>15</v>
       </c>
       <c r="AM2" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AN2" s="9" t="s">
+      <c r="AO2" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" s="21">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="4">
@@ -1346,13 +1359,20 @@
       <c r="AJ3" s="7">
         <v>2000</v>
       </c>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="7"/>
-      <c r="AM3" s="4"/>
-      <c r="AN3" s="7"/>
+      <c r="AK3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AL3" s="7">
+        <v>7</v>
+      </c>
+      <c r="AM3" s="10">
+        <v>15</v>
+      </c>
+      <c r="AN3" s="4"/>
+      <c r="AO3" s="7"/>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A4" s="21">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
       <c r="B4" s="4">
@@ -1460,12 +1480,15 @@
       <c r="AJ4" s="7">
         <v>1000</v>
       </c>
-      <c r="AK4" s="4"/>
+      <c r="AK4" s="4">
+        <v>60</v>
+      </c>
       <c r="AL4" s="7"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="7"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="4"/>
+      <c r="AO4" s="7"/>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5" s="14">
         <v>3</v>
       </c>
@@ -1576,10 +1599,11 @@
       </c>
       <c r="AK5" s="4"/>
       <c r="AL5" s="7"/>
-      <c r="AM5" s="4"/>
-      <c r="AN5" s="7"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="4"/>
+      <c r="AO5" s="7"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>4</v>
       </c>
@@ -1690,10 +1714,11 @@
       </c>
       <c r="AK6" s="4"/>
       <c r="AL6" s="7"/>
-      <c r="AM6" s="4"/>
-      <c r="AN6" s="7"/>
+      <c r="AM6" s="5"/>
+      <c r="AN6" s="4"/>
+      <c r="AO6" s="7"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>5</v>
       </c>
@@ -1796,11 +1821,12 @@
       </c>
       <c r="AK7" s="4"/>
       <c r="AL7" s="7"/>
-      <c r="AM7" s="4"/>
-      <c r="AN7" s="7"/>
-      <c r="AO7"/>
+      <c r="AM7" s="5"/>
+      <c r="AN7" s="4"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>6</v>
       </c>
@@ -1911,10 +1937,11 @@
       </c>
       <c r="AK8" s="4"/>
       <c r="AL8" s="7"/>
-      <c r="AM8" s="4"/>
-      <c r="AN8" s="7"/>
+      <c r="AM8" s="5"/>
+      <c r="AN8" s="4"/>
+      <c r="AO8" s="7"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>7</v>
       </c>
@@ -2025,10 +2052,11 @@
       </c>
       <c r="AK9" s="4"/>
       <c r="AL9" s="7"/>
-      <c r="AM9" s="4"/>
-      <c r="AN9" s="7"/>
+      <c r="AM9" s="5"/>
+      <c r="AN9" s="4"/>
+      <c r="AO9" s="7"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2139,10 +2167,11 @@
       </c>
       <c r="AK10" s="4"/>
       <c r="AL10" s="7"/>
-      <c r="AM10" s="4"/>
-      <c r="AN10" s="7"/>
+      <c r="AM10" s="5"/>
+      <c r="AN10" s="4"/>
+      <c r="AO10" s="7"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2245,10 +2274,11 @@
       </c>
       <c r="AK11" s="4"/>
       <c r="AL11" s="7"/>
-      <c r="AM11" s="4"/>
-      <c r="AN11" s="7"/>
+      <c r="AM11" s="5"/>
+      <c r="AN11" s="4"/>
+      <c r="AO11" s="7"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2351,10 +2381,11 @@
       </c>
       <c r="AK12" s="4"/>
       <c r="AL12" s="7"/>
-      <c r="AM12" s="4"/>
-      <c r="AN12" s="7"/>
+      <c r="AM12" s="5"/>
+      <c r="AN12" s="4"/>
+      <c r="AO12" s="7"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2465,10 +2496,11 @@
       </c>
       <c r="AK13" s="4"/>
       <c r="AL13" s="7"/>
-      <c r="AM13" s="4"/>
-      <c r="AN13" s="7"/>
+      <c r="AM13" s="5"/>
+      <c r="AN13" s="4"/>
+      <c r="AO13" s="7"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2571,10 +2603,11 @@
       </c>
       <c r="AK14" s="4"/>
       <c r="AL14" s="7"/>
-      <c r="AM14" s="4"/>
-      <c r="AN14" s="7"/>
+      <c r="AM14" s="5"/>
+      <c r="AN14" s="4"/>
+      <c r="AO14" s="7"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2685,10 +2718,11 @@
       </c>
       <c r="AK15" s="4"/>
       <c r="AL15" s="7"/>
-      <c r="AM15" s="4"/>
-      <c r="AN15" s="7"/>
+      <c r="AM15" s="5"/>
+      <c r="AN15" s="4"/>
+      <c r="AO15" s="7"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2799,10 +2833,11 @@
       </c>
       <c r="AK16" s="4"/>
       <c r="AL16" s="7"/>
-      <c r="AM16" s="4"/>
-      <c r="AN16" s="7"/>
+      <c r="AM16" s="5"/>
+      <c r="AN16" s="4"/>
+      <c r="AO16" s="7"/>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2913,10 +2948,11 @@
       </c>
       <c r="AK17" s="4"/>
       <c r="AL17" s="7"/>
-      <c r="AM17" s="4"/>
-      <c r="AN17" s="7"/>
+      <c r="AM17" s="5"/>
+      <c r="AN17" s="4"/>
+      <c r="AO17" s="7"/>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3027,10 +3063,11 @@
       </c>
       <c r="AK18" s="4"/>
       <c r="AL18" s="7"/>
-      <c r="AM18" s="4"/>
-      <c r="AN18" s="7"/>
+      <c r="AM18" s="5"/>
+      <c r="AN18" s="4"/>
+      <c r="AO18" s="7"/>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3141,10 +3178,11 @@
       </c>
       <c r="AK19" s="4"/>
       <c r="AL19" s="7"/>
-      <c r="AM19" s="4"/>
-      <c r="AN19" s="7"/>
+      <c r="AM19" s="5"/>
+      <c r="AN19" s="4"/>
+      <c r="AO19" s="7"/>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3255,10 +3293,11 @@
       </c>
       <c r="AK20" s="4"/>
       <c r="AL20" s="7"/>
-      <c r="AM20" s="4"/>
-      <c r="AN20" s="7"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="4"/>
+      <c r="AO20" s="7"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3369,10 +3408,11 @@
       </c>
       <c r="AK21" s="4"/>
       <c r="AL21" s="7"/>
-      <c r="AM21" s="4"/>
-      <c r="AN21" s="7"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="4"/>
+      <c r="AO21" s="7"/>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -3482,7 +3522,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -3594,6 +3634,8 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AN1:AO1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="G1:K1"/>
     <mergeCell ref="AF1:AJ1"/>
@@ -3602,8 +3644,6 @@
     <mergeCell ref="AA1:AE1"/>
     <mergeCell ref="V1:Z1"/>
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="AK1:AL1"/>
-    <mergeCell ref="AM1:AN1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
changes to config file
</commit_message>
<xml_diff>
--- a/Configurations.xlsx
+++ b/Configurations.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23524"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cce1d1199b24a628/Code/DE Assignments/Configuration YAMLs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="91" documentId="14_{0C773CF9-0358-4C32-AC23-85F757E65E78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FD158E6A-AD10-44AD-B82C-F84C2095E391}"/>
+  <xr:revisionPtr revIDLastSave="297" documentId="14_{0C773CF9-0358-4C32-AC23-85F757E65E78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B754B224-B404-4D4B-894D-EEFCC78BD3FC}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -33,7 +33,43 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="29">
   <si>
+    <t>Test No</t>
+  </si>
+  <si>
+    <t>Configuration no</t>
+  </si>
+  <si>
+    <t>DB</t>
+  </si>
+  <si>
     <t>Registry</t>
+  </si>
+  <si>
+    <t>Persistence</t>
+  </si>
+  <si>
+    <t>Auth</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Recommender</t>
+  </si>
+  <si>
+    <t>WebUI</t>
+  </si>
+  <si>
+    <t>Load Config</t>
+  </si>
+  <si>
+    <t>Performance highlights</t>
+  </si>
+  <si>
+    <t>Timing</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
   <si>
     <t>No. of Replicas</t>
@@ -51,70 +87,34 @@
     <t>CPU Limits</t>
   </si>
   <si>
-    <t>WebUI</t>
-  </si>
-  <si>
-    <t>Auth</t>
-  </si>
-  <si>
-    <t>Persistence</t>
-  </si>
-  <si>
-    <t>Recommender</t>
-  </si>
-  <si>
-    <t>Image</t>
-  </si>
-  <si>
-    <t>DB</t>
-  </si>
-  <si>
-    <t>Load Config</t>
-  </si>
-  <si>
     <t>No. of users</t>
   </si>
   <si>
     <t>Ramp up time</t>
   </si>
   <si>
-    <t>Timing</t>
+    <t>Total time</t>
+  </si>
+  <si>
+    <t>Configuration viable?</t>
+  </si>
+  <si>
+    <t>No. of Nodes</t>
+  </si>
+  <si>
+    <t>Average error rate</t>
   </si>
   <si>
     <t>Time started</t>
   </si>
   <si>
-    <t>Total time</t>
-  </si>
-  <si>
-    <t>Test No</t>
-  </si>
-  <si>
-    <t>Configuration no</t>
-  </si>
-  <si>
-    <t>Configuration viable?</t>
-  </si>
-  <si>
-    <t>Notes</t>
+    <t>0.25Gi</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>0.25Gi</t>
-  </si>
-  <si>
     <t>0.5Gi</t>
-  </si>
-  <si>
-    <t>Average error rate</t>
-  </si>
-  <si>
-    <t>Performance highlights</t>
-  </si>
-  <si>
-    <t>No. of Nodes</t>
   </si>
   <si>
     <t>No</t>
@@ -124,7 +124,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -824,9 +824,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -890,6 +887,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="37" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1279,12 +1279,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="7" ySplit="17" topLeftCell="AL38" activePane="bottomRight" state="frozen"/>
+      <selection pane="bottomRight" activeCell="AS44" sqref="AS44"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A18"/>
-      <selection pane="bottomRight" activeCell="AS44" sqref="AS44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="10.42578125" style="1" customWidth="1"/>
@@ -1299,349 +1299,349 @@
     <col min="47" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" ht="35.25" customHeight="1">
       <c r="A1" s="55" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="62" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C1" s="59" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" s="59"/>
       <c r="E1" s="59"/>
       <c r="F1" s="59"/>
       <c r="G1" s="59"/>
       <c r="H1" s="64" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I1" s="64"/>
       <c r="J1" s="64"/>
       <c r="K1" s="64"/>
       <c r="L1" s="64"/>
       <c r="M1" s="59" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="N1" s="59"/>
       <c r="O1" s="59"/>
       <c r="P1" s="59"/>
       <c r="Q1" s="59"/>
       <c r="R1" s="59" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="S1" s="59"/>
       <c r="T1" s="59"/>
       <c r="U1" s="59"/>
       <c r="V1" s="59"/>
       <c r="W1" s="59" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="X1" s="59"/>
       <c r="Y1" s="59"/>
       <c r="Z1" s="59"/>
       <c r="AA1" s="59"/>
       <c r="AB1" s="59" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AC1" s="59"/>
       <c r="AD1" s="59"/>
       <c r="AE1" s="59"/>
       <c r="AF1" s="59"/>
       <c r="AG1" s="64" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AH1" s="64"/>
       <c r="AI1" s="64"/>
       <c r="AJ1" s="64"/>
       <c r="AK1" s="64"/>
       <c r="AL1" s="59" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AM1" s="59"/>
-      <c r="AN1" s="15"/>
+      <c r="AN1" s="54"/>
       <c r="AO1" s="56" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="AP1" s="57"/>
       <c r="AQ1" s="58"/>
       <c r="AR1" s="60" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="AS1" s="61"/>
       <c r="AT1" s="1" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:46" ht="45.75" thickBot="1">
       <c r="A2" s="55"/>
       <c r="B2" s="63"/>
       <c r="C2" s="8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="S2" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="W2" s="8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="X2" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="Y2" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="Z2" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="AA2" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="AB2" s="8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AC2" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="AD2" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AE2" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="AF2" s="8" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="AG2" s="8" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="AH2" s="8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="AI2" s="8" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="AJ2" s="8" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="AK2" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="AL2" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM2" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="AN2" s="22" t="s">
         <v>17</v>
       </c>
+      <c r="AL2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM2" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="AN2" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="AO2" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AP2" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ2" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="AS2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AP2" s="52" t="s">
-        <v>27</v>
-      </c>
-      <c r="AQ2" s="23" t="s">
+    </row>
+    <row r="3" spans="1:46">
+      <c r="A3" s="23">
+        <v>1</v>
+      </c>
+      <c r="B3" s="24">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25">
+        <v>1</v>
+      </c>
+      <c r="D3" s="26">
+        <v>0.2</v>
+      </c>
+      <c r="E3" s="26">
+        <v>1</v>
+      </c>
+      <c r="F3" s="26">
+        <v>0.1</v>
+      </c>
+      <c r="G3" s="27">
+        <v>1</v>
+      </c>
+      <c r="H3" s="28">
+        <v>2</v>
+      </c>
+      <c r="I3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="AR2" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="AS2" s="9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="24">
-        <v>1</v>
-      </c>
-      <c r="B3" s="25">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26">
-        <v>1</v>
-      </c>
-      <c r="D3" s="27">
+      <c r="J3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="26">
+        <v>0.01</v>
+      </c>
+      <c r="L3" s="29">
+        <v>1</v>
+      </c>
+      <c r="M3" s="25">
+        <v>1</v>
+      </c>
+      <c r="N3" s="26">
+        <v>0.6</v>
+      </c>
+      <c r="O3" s="26">
+        <v>1</v>
+      </c>
+      <c r="P3" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Q3" s="27">
+        <v>1</v>
+      </c>
+      <c r="R3" s="25">
+        <v>2</v>
+      </c>
+      <c r="S3" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="T3" s="26">
+        <v>1</v>
+      </c>
+      <c r="U3" s="26">
         <v>0.2</v>
       </c>
-      <c r="E3" s="27">
-        <v>1</v>
-      </c>
-      <c r="F3" s="27">
-        <v>0.1</v>
-      </c>
-      <c r="G3" s="28">
-        <v>1</v>
-      </c>
-      <c r="H3" s="29">
-        <v>2</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="27">
-        <v>0.01</v>
-      </c>
-      <c r="L3" s="30">
-        <v>1</v>
-      </c>
-      <c r="M3" s="26">
-        <v>1</v>
-      </c>
-      <c r="N3" s="27">
-        <v>0.6</v>
-      </c>
-      <c r="O3" s="27">
-        <v>1</v>
-      </c>
-      <c r="P3" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="Q3" s="28">
-        <v>1</v>
-      </c>
-      <c r="R3" s="26">
-        <v>2</v>
-      </c>
-      <c r="S3" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="T3" s="27">
-        <v>1</v>
-      </c>
-      <c r="U3" s="27">
-        <v>0.2</v>
-      </c>
-      <c r="V3" s="28">
-        <v>1</v>
-      </c>
-      <c r="W3" s="26">
-        <v>1</v>
-      </c>
-      <c r="X3" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="Y3" s="27">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="27">
+      <c r="V3" s="27">
+        <v>1</v>
+      </c>
+      <c r="W3" s="25">
+        <v>1</v>
+      </c>
+      <c r="X3" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="Y3" s="26">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="26">
         <v>0.3</v>
       </c>
-      <c r="AA3" s="30">
-        <v>2</v>
-      </c>
-      <c r="AB3" s="26">
+      <c r="AA3" s="29">
+        <v>2</v>
+      </c>
+      <c r="AB3" s="25">
         <v>0</v>
       </c>
-      <c r="AC3" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD3" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE3" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF3" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG3" s="29">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="27">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="27">
-        <v>2</v>
-      </c>
-      <c r="AJ3" s="27">
-        <v>0.5</v>
-      </c>
-      <c r="AK3" s="31">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="26">
+      <c r="AC3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE3" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF3" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG3" s="28">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="26">
+        <v>1</v>
+      </c>
+      <c r="AI3" s="26">
+        <v>2</v>
+      </c>
+      <c r="AJ3" s="26">
+        <v>0.5</v>
+      </c>
+      <c r="AK3" s="30">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="25">
         <v>50</v>
       </c>
-      <c r="AM3" s="31">
+      <c r="AM3" s="30">
         <v>600</v>
       </c>
-      <c r="AN3" s="28">
+      <c r="AN3" s="27">
         <v>1200</v>
       </c>
-      <c r="AO3" s="20"/>
-      <c r="AP3" s="37">
+      <c r="AO3" s="19"/>
+      <c r="AP3" s="36">
         <v>8</v>
       </c>
       <c r="AQ3" s="10"/>
       <c r="AR3" s="4"/>
-      <c r="AS3" s="53">
+      <c r="AS3" s="52">
         <v>0.84236111111111101</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="16"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="4"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
@@ -1692,11 +1692,11 @@
       </c>
       <c r="AQ4" s="10"/>
       <c r="AR4" s="4"/>
-      <c r="AS4" s="53">
+      <c r="AS4" s="52">
         <v>0.83680555555555547</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1751,142 +1751,142 @@
       </c>
       <c r="AQ5" s="10"/>
       <c r="AR5" s="4"/>
-      <c r="AS5" s="53">
+      <c r="AS5" s="52">
         <v>0.84652777777777777</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
+    <row r="6" spans="1:46">
+      <c r="A6" s="31">
         <v>4</v>
       </c>
-      <c r="B6" s="33">
-        <v>2</v>
-      </c>
-      <c r="C6" s="34">
-        <v>2</v>
-      </c>
-      <c r="D6" s="32">
+      <c r="B6" s="32">
+        <v>2</v>
+      </c>
+      <c r="C6" s="33">
+        <v>2</v>
+      </c>
+      <c r="D6" s="31">
         <v>0.1</v>
       </c>
-      <c r="E6" s="32">
-        <v>2</v>
-      </c>
-      <c r="F6" s="32">
+      <c r="E6" s="31">
+        <v>2</v>
+      </c>
+      <c r="F6" s="31">
         <v>0.05</v>
       </c>
-      <c r="G6" s="35">
-        <v>1</v>
-      </c>
-      <c r="H6" s="34">
-        <v>1</v>
-      </c>
-      <c r="I6" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="36" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="36">
+      <c r="G6" s="34">
+        <v>1</v>
+      </c>
+      <c r="H6" s="33">
+        <v>1</v>
+      </c>
+      <c r="I6" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="K6" s="35">
         <v>0.02</v>
       </c>
-      <c r="L6" s="35">
+      <c r="L6" s="34">
         <v>0.15</v>
       </c>
-      <c r="M6" s="34">
-        <v>1</v>
-      </c>
-      <c r="N6" s="36">
+      <c r="M6" s="33">
+        <v>1</v>
+      </c>
+      <c r="N6" s="35">
         <v>0.6</v>
       </c>
-      <c r="O6" s="36">
-        <v>1</v>
-      </c>
-      <c r="P6" s="36">
+      <c r="O6" s="35">
+        <v>1</v>
+      </c>
+      <c r="P6" s="35">
         <v>0.6</v>
       </c>
-      <c r="Q6" s="35">
+      <c r="Q6" s="34">
         <v>0.6</v>
       </c>
-      <c r="R6" s="34">
-        <v>1</v>
-      </c>
-      <c r="S6" s="36">
-        <v>1</v>
-      </c>
-      <c r="T6" s="36">
-        <v>2</v>
-      </c>
-      <c r="U6" s="36">
+      <c r="R6" s="33">
+        <v>1</v>
+      </c>
+      <c r="S6" s="35">
+        <v>1</v>
+      </c>
+      <c r="T6" s="35">
+        <v>2</v>
+      </c>
+      <c r="U6" s="35">
         <v>0.4</v>
       </c>
-      <c r="V6" s="35">
-        <v>1</v>
-      </c>
-      <c r="W6" s="34">
-        <v>1</v>
-      </c>
-      <c r="X6" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="Y6" s="32">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="32">
+      <c r="V6" s="34">
+        <v>1</v>
+      </c>
+      <c r="W6" s="33">
+        <v>1</v>
+      </c>
+      <c r="X6" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="Y6" s="31">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="31">
         <v>0.4</v>
       </c>
-      <c r="AA6" s="35">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="34">
-        <v>2</v>
-      </c>
-      <c r="AC6" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="AD6" s="36">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="36">
+      <c r="AA6" s="34">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="33">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="AD6" s="35">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="35">
         <v>0.1</v>
       </c>
-      <c r="AF6" s="35">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="34">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="36">
-        <v>0.5</v>
-      </c>
-      <c r="AI6" s="36">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="36">
+      <c r="AF6" s="34">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="33">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="AI6" s="35">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="35">
         <v>0.6</v>
       </c>
-      <c r="AK6" s="32">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="34">
+      <c r="AK6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="33">
         <v>50</v>
       </c>
-      <c r="AM6" s="32">
+      <c r="AM6" s="31">
         <v>600</v>
       </c>
-      <c r="AN6" s="35">
+      <c r="AN6" s="34">
         <v>1200</v>
       </c>
       <c r="AO6" s="13"/>
-      <c r="AP6" s="32">
+      <c r="AP6" s="31">
         <v>8</v>
       </c>
       <c r="AQ6" s="10"/>
       <c r="AR6" s="4"/>
-      <c r="AS6" s="51">
+      <c r="AS6" s="50">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46">
       <c r="A7" s="10">
         <v>5</v>
       </c>
@@ -1941,12 +1941,12 @@
       </c>
       <c r="AQ7" s="10"/>
       <c r="AR7" s="4"/>
-      <c r="AS7" s="51">
+      <c r="AS7" s="50">
         <v>0.83958333333333324</v>
       </c>
       <c r="AT7"/>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46">
       <c r="A8" s="10">
         <v>6</v>
       </c>
@@ -2001,142 +2001,142 @@
       </c>
       <c r="AQ8" s="10"/>
       <c r="AR8" s="4"/>
-      <c r="AS8" s="51">
+      <c r="AS8" s="50">
         <v>0.84305555555555556</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="37">
+    <row r="9" spans="1:46">
+      <c r="A9" s="36">
         <v>7</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="23">
         <v>3</v>
       </c>
-      <c r="C9" s="38">
-        <v>1</v>
-      </c>
-      <c r="D9" s="37">
+      <c r="C9" s="37">
+        <v>1</v>
+      </c>
+      <c r="D9" s="36">
         <v>0.2</v>
       </c>
-      <c r="E9" s="37">
-        <v>2</v>
-      </c>
-      <c r="F9" s="37">
+      <c r="E9" s="36">
+        <v>2</v>
+      </c>
+      <c r="F9" s="36">
         <v>0.1</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="38">
         <v>0.1</v>
       </c>
-      <c r="H9" s="38">
-        <v>2</v>
-      </c>
-      <c r="I9" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K9" s="40">
+      <c r="H9" s="37">
+        <v>2</v>
+      </c>
+      <c r="I9" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K9" s="39">
         <v>0.01</v>
       </c>
-      <c r="L9" s="39">
-        <v>1</v>
-      </c>
-      <c r="M9" s="38">
-        <v>1</v>
-      </c>
-      <c r="N9" s="40">
+      <c r="L9" s="38">
+        <v>1</v>
+      </c>
+      <c r="M9" s="37">
+        <v>1</v>
+      </c>
+      <c r="N9" s="39">
         <v>0.6</v>
       </c>
-      <c r="O9" s="40">
-        <v>1</v>
-      </c>
-      <c r="P9" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="Q9" s="39">
+      <c r="O9" s="39">
+        <v>1</v>
+      </c>
+      <c r="P9" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="Q9" s="38">
         <v>0.6</v>
       </c>
-      <c r="R9" s="38">
-        <v>2</v>
-      </c>
-      <c r="S9" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="T9" s="40">
-        <v>1</v>
-      </c>
-      <c r="U9" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="V9" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="W9" s="38">
-        <v>1</v>
-      </c>
-      <c r="X9" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="Y9" s="37">
-        <v>2</v>
-      </c>
-      <c r="Z9" s="37">
+      <c r="R9" s="37">
+        <v>2</v>
+      </c>
+      <c r="S9" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="T9" s="39">
+        <v>1</v>
+      </c>
+      <c r="U9" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="V9" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="W9" s="37">
+        <v>1</v>
+      </c>
+      <c r="X9" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Y9" s="36">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="36">
         <v>0.3</v>
       </c>
-      <c r="AA9" s="39">
-        <v>2</v>
-      </c>
-      <c r="AB9" s="38">
+      <c r="AA9" s="38">
+        <v>2</v>
+      </c>
+      <c r="AB9" s="37">
         <v>0</v>
       </c>
-      <c r="AC9" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD9" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE9" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF9" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG9" s="38">
-        <v>1</v>
-      </c>
-      <c r="AH9" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="AI9" s="40">
-        <v>1</v>
-      </c>
-      <c r="AJ9" s="40">
-        <v>0.5</v>
-      </c>
-      <c r="AK9" s="37">
-        <v>1</v>
-      </c>
-      <c r="AL9" s="38">
+      <c r="AC9" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD9" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE9" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF9" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG9" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="AI9" s="39">
+        <v>1</v>
+      </c>
+      <c r="AJ9" s="39">
+        <v>0.5</v>
+      </c>
+      <c r="AK9" s="36">
+        <v>1</v>
+      </c>
+      <c r="AL9" s="37">
         <v>50</v>
       </c>
-      <c r="AM9" s="37">
+      <c r="AM9" s="36">
         <v>600</v>
       </c>
-      <c r="AN9" s="39">
+      <c r="AN9" s="38">
         <v>1200</v>
       </c>
       <c r="AO9" s="13"/>
-      <c r="AP9" s="32">
+      <c r="AP9" s="31">
         <v>8</v>
       </c>
       <c r="AQ9" s="10"/>
       <c r="AR9" s="4"/>
-      <c r="AS9" s="51">
+      <c r="AS9" s="50">
         <v>0.84097222222222223</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2190,11 +2190,11 @@
       </c>
       <c r="AQ10" s="10"/>
       <c r="AR10" s="4"/>
-      <c r="AS10" s="51">
+      <c r="AS10" s="50">
         <v>0.84027777777777779</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2248,142 +2248,142 @@
       </c>
       <c r="AQ11" s="10"/>
       <c r="AR11" s="4"/>
-      <c r="AS11" s="51">
+      <c r="AS11" s="50">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="41">
+    <row r="12" spans="1:46">
+      <c r="A12" s="40">
         <v>10</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="40">
         <v>4</v>
       </c>
-      <c r="C12" s="42">
-        <v>2</v>
-      </c>
-      <c r="D12" s="43">
+      <c r="C12" s="41">
+        <v>2</v>
+      </c>
+      <c r="D12" s="42">
         <v>0.1</v>
       </c>
-      <c r="E12" s="43">
-        <v>2</v>
-      </c>
-      <c r="F12" s="43">
+      <c r="E12" s="42">
+        <v>2</v>
+      </c>
+      <c r="F12" s="42">
         <v>0.05</v>
       </c>
-      <c r="G12" s="44">
-        <v>1</v>
-      </c>
-      <c r="H12" s="42">
-        <v>1</v>
-      </c>
-      <c r="I12" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="K12" s="43">
+      <c r="G12" s="43">
+        <v>1</v>
+      </c>
+      <c r="H12" s="41">
+        <v>1</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="K12" s="42">
         <v>0.02</v>
       </c>
-      <c r="L12" s="44">
+      <c r="L12" s="43">
         <v>0.15</v>
       </c>
-      <c r="M12" s="42">
-        <v>1</v>
-      </c>
-      <c r="N12" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="O12" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="P12" s="43">
+      <c r="M12" s="41">
+        <v>1</v>
+      </c>
+      <c r="N12" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="O12" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="42">
         <v>0.6</v>
       </c>
-      <c r="Q12" s="44">
+      <c r="Q12" s="43">
         <v>0.6</v>
       </c>
-      <c r="R12" s="42">
-        <v>1</v>
-      </c>
-      <c r="S12" s="43">
-        <v>1</v>
-      </c>
-      <c r="T12" s="43">
-        <v>2</v>
-      </c>
-      <c r="U12" s="43">
+      <c r="R12" s="41">
+        <v>1</v>
+      </c>
+      <c r="S12" s="42">
+        <v>1</v>
+      </c>
+      <c r="T12" s="42">
+        <v>2</v>
+      </c>
+      <c r="U12" s="42">
         <v>0.4</v>
       </c>
-      <c r="V12" s="44">
-        <v>1</v>
-      </c>
-      <c r="W12" s="42">
-        <v>1</v>
-      </c>
-      <c r="X12" s="43">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="43">
-        <v>1</v>
-      </c>
-      <c r="Z12" s="43">
+      <c r="V12" s="43">
+        <v>1</v>
+      </c>
+      <c r="W12" s="41">
+        <v>1</v>
+      </c>
+      <c r="X12" s="42">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="42">
+        <v>1</v>
+      </c>
+      <c r="Z12" s="42">
         <v>0.4</v>
       </c>
-      <c r="AA12" s="44">
-        <v>1</v>
-      </c>
-      <c r="AB12" s="42">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="43">
+      <c r="AA12" s="43">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="41">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="42">
         <v>0.6</v>
       </c>
-      <c r="AD12" s="43">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="43">
+      <c r="AD12" s="42">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="42">
         <v>0.2</v>
       </c>
-      <c r="AF12" s="44">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="42">
-        <v>1</v>
-      </c>
-      <c r="AH12" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="AI12" s="43">
-        <v>2</v>
-      </c>
-      <c r="AJ12" s="43">
-        <v>0.5</v>
-      </c>
-      <c r="AK12" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="AL12" s="42">
+      <c r="AF12" s="43">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="41">
+        <v>1</v>
+      </c>
+      <c r="AH12" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="AI12" s="42">
+        <v>2</v>
+      </c>
+      <c r="AJ12" s="42">
+        <v>0.5</v>
+      </c>
+      <c r="AK12" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="AL12" s="41">
         <v>50</v>
       </c>
-      <c r="AM12" s="45">
+      <c r="AM12" s="44">
         <v>600</v>
       </c>
-      <c r="AN12" s="44">
+      <c r="AN12" s="43">
         <v>1200</v>
       </c>
       <c r="AO12" s="13"/>
-      <c r="AP12" s="45">
+      <c r="AP12" s="44">
         <v>8</v>
       </c>
       <c r="AQ12" s="10"/>
       <c r="AR12" s="4"/>
-      <c r="AS12" s="51">
+      <c r="AS12" s="50">
         <v>0.8534722222222223</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46">
       <c r="A13" s="10">
         <v>11</v>
       </c>
@@ -2435,11 +2435,11 @@
       <c r="AP13" s="10"/>
       <c r="AQ13" s="10"/>
       <c r="AR13" s="4"/>
-      <c r="AS13" s="51">
+      <c r="AS13" s="50">
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46">
       <c r="A14" s="10">
         <v>12</v>
       </c>
@@ -2491,140 +2491,140 @@
       <c r="AP14" s="10"/>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="4"/>
-      <c r="AS14" s="51">
+      <c r="AS14" s="50">
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="37">
+    <row r="15" spans="1:46">
+      <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="23">
         <v>5</v>
       </c>
-      <c r="C15" s="38">
-        <v>1</v>
-      </c>
-      <c r="D15" s="37">
+      <c r="C15" s="37">
+        <v>1</v>
+      </c>
+      <c r="D15" s="36">
         <v>0.1</v>
       </c>
-      <c r="E15" s="37">
-        <v>1</v>
-      </c>
-      <c r="F15" s="37">
+      <c r="E15" s="36">
+        <v>1</v>
+      </c>
+      <c r="F15" s="36">
         <v>0.05</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="38">
         <v>0.1</v>
       </c>
-      <c r="H15" s="38">
-        <v>1</v>
-      </c>
-      <c r="I15" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="40" t="s">
-        <v>23</v>
-      </c>
-      <c r="K15" s="37">
+      <c r="H15" s="37">
+        <v>1</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="36">
         <v>0.01</v>
       </c>
-      <c r="L15" s="39">
+      <c r="L15" s="38">
         <v>0.15</v>
       </c>
-      <c r="M15" s="38">
-        <v>1</v>
-      </c>
-      <c r="N15" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="O15" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="P15" s="37">
+      <c r="M15" s="37">
+        <v>1</v>
+      </c>
+      <c r="N15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="O15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P15" s="36">
         <v>0.6</v>
       </c>
-      <c r="Q15" s="39">
-        <v>1</v>
-      </c>
-      <c r="R15" s="38">
-        <v>1</v>
-      </c>
-      <c r="S15" s="37">
-        <v>1</v>
-      </c>
-      <c r="T15" s="37">
-        <v>2</v>
-      </c>
-      <c r="U15" s="37">
+      <c r="Q15" s="38">
+        <v>1</v>
+      </c>
+      <c r="R15" s="37">
+        <v>1</v>
+      </c>
+      <c r="S15" s="36">
+        <v>1</v>
+      </c>
+      <c r="T15" s="36">
+        <v>2</v>
+      </c>
+      <c r="U15" s="36">
         <v>0.4</v>
       </c>
-      <c r="V15" s="39">
-        <v>1</v>
-      </c>
-      <c r="W15" s="38">
-        <v>1</v>
-      </c>
-      <c r="X15" s="37">
-        <v>1</v>
-      </c>
-      <c r="Y15" s="37">
-        <v>1</v>
-      </c>
-      <c r="Z15" s="37">
+      <c r="V15" s="38">
+        <v>1</v>
+      </c>
+      <c r="W15" s="37">
+        <v>1</v>
+      </c>
+      <c r="X15" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y15" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z15" s="36">
         <v>0.4</v>
       </c>
-      <c r="AA15" s="39">
-        <v>1</v>
-      </c>
-      <c r="AB15" s="38">
-        <v>1</v>
-      </c>
-      <c r="AC15" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AD15" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AE15" s="37">
+      <c r="AA15" s="38">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="37">
+        <v>1</v>
+      </c>
+      <c r="AC15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AD15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AE15" s="36">
         <v>0.1</v>
       </c>
-      <c r="AF15" s="39">
-        <v>1</v>
-      </c>
-      <c r="AG15" s="38">
-        <v>1</v>
-      </c>
-      <c r="AH15" s="37">
-        <v>1</v>
-      </c>
-      <c r="AI15" s="37">
-        <v>1</v>
-      </c>
-      <c r="AJ15" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AK15" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AL15" s="38">
+      <c r="AF15" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH15" s="36">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AK15" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AL15" s="37">
         <v>50</v>
       </c>
-      <c r="AM15" s="37">
+      <c r="AM15" s="36">
         <v>600</v>
       </c>
-      <c r="AN15" s="39">
+      <c r="AN15" s="38">
         <v>1200</v>
       </c>
       <c r="AO15" s="13"/>
       <c r="AP15" s="10"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="4"/>
-      <c r="AS15" s="51">
+      <c r="AS15" s="50">
         <v>0.8354166666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46">
       <c r="A16" s="10">
         <v>14</v>
       </c>
@@ -2676,11 +2676,11 @@
       <c r="AP16" s="10"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="4"/>
-      <c r="AS16" s="51">
+      <c r="AS16" s="50">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:45">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2732,140 +2732,140 @@
       <c r="AP17" s="10"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="4"/>
-      <c r="AS17" s="51">
+      <c r="AS17" s="50">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A18" s="41">
+    <row r="18" spans="1:45">
+      <c r="A18" s="40">
         <v>16</v>
       </c>
-      <c r="B18" s="41">
+      <c r="B18" s="40">
         <v>6</v>
       </c>
-      <c r="C18" s="42">
-        <v>2</v>
-      </c>
-      <c r="D18" s="45">
+      <c r="C18" s="41">
+        <v>2</v>
+      </c>
+      <c r="D18" s="44">
         <v>0.2</v>
       </c>
-      <c r="E18" s="45">
-        <v>1</v>
-      </c>
-      <c r="F18" s="45">
+      <c r="E18" s="44">
+        <v>1</v>
+      </c>
+      <c r="F18" s="44">
         <v>0.1</v>
       </c>
-      <c r="G18" s="44">
+      <c r="G18" s="43">
         <v>0.1</v>
       </c>
-      <c r="H18" s="42">
-        <v>2</v>
-      </c>
-      <c r="I18" s="43" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="K18" s="45">
+      <c r="H18" s="41">
+        <v>2</v>
+      </c>
+      <c r="I18" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="44">
         <v>0.01</v>
       </c>
-      <c r="L18" s="44">
-        <v>1</v>
-      </c>
-      <c r="M18" s="42">
-        <v>1</v>
-      </c>
-      <c r="N18" s="45">
+      <c r="L18" s="43">
+        <v>1</v>
+      </c>
+      <c r="M18" s="41">
+        <v>1</v>
+      </c>
+      <c r="N18" s="44">
         <v>0.6</v>
       </c>
-      <c r="O18" s="45">
-        <v>1</v>
-      </c>
-      <c r="P18" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="Q18" s="44">
-        <v>1</v>
-      </c>
-      <c r="R18" s="42">
-        <v>2</v>
-      </c>
-      <c r="S18" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="T18" s="45">
-        <v>1</v>
-      </c>
-      <c r="U18" s="45">
+      <c r="O18" s="44">
+        <v>1</v>
+      </c>
+      <c r="P18" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="Q18" s="43">
+        <v>1</v>
+      </c>
+      <c r="R18" s="41">
+        <v>2</v>
+      </c>
+      <c r="S18" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="T18" s="44">
+        <v>1</v>
+      </c>
+      <c r="U18" s="44">
         <v>0.2</v>
       </c>
-      <c r="V18" s="44">
-        <v>0.5</v>
-      </c>
-      <c r="W18" s="42">
-        <v>1</v>
-      </c>
-      <c r="X18" s="45">
-        <v>1</v>
-      </c>
-      <c r="Y18" s="45">
-        <v>2</v>
-      </c>
-      <c r="Z18" s="45">
+      <c r="V18" s="43">
+        <v>0.5</v>
+      </c>
+      <c r="W18" s="41">
+        <v>1</v>
+      </c>
+      <c r="X18" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y18" s="44">
+        <v>2</v>
+      </c>
+      <c r="Z18" s="44">
         <v>0.3</v>
       </c>
-      <c r="AA18" s="44">
-        <v>2</v>
-      </c>
-      <c r="AB18" s="42">
-        <v>2</v>
-      </c>
-      <c r="AC18" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="AD18" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="AE18" s="45">
+      <c r="AA18" s="43">
+        <v>2</v>
+      </c>
+      <c r="AB18" s="41">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="AD18" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="AE18" s="44">
         <v>0.2</v>
       </c>
-      <c r="AF18" s="44">
+      <c r="AF18" s="43">
         <v>0.25</v>
       </c>
-      <c r="AG18" s="42">
-        <v>1</v>
-      </c>
-      <c r="AH18" s="45">
-        <v>1</v>
-      </c>
-      <c r="AI18" s="45">
-        <v>2</v>
-      </c>
-      <c r="AJ18" s="45">
+      <c r="AG18" s="41">
+        <v>1</v>
+      </c>
+      <c r="AH18" s="44">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="44">
+        <v>2</v>
+      </c>
+      <c r="AJ18" s="44">
         <v>0.6</v>
       </c>
-      <c r="AK18" s="45">
-        <v>1</v>
-      </c>
-      <c r="AL18" s="42">
+      <c r="AK18" s="44">
+        <v>1</v>
+      </c>
+      <c r="AL18" s="41">
         <v>50</v>
       </c>
-      <c r="AM18" s="45">
+      <c r="AM18" s="44">
         <v>600</v>
       </c>
-      <c r="AN18" s="44">
+      <c r="AN18" s="43">
         <v>1200</v>
       </c>
       <c r="AO18" s="13"/>
       <c r="AP18" s="10"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="4"/>
-      <c r="AS18" s="51">
+      <c r="AS18" s="50">
         <v>0.84375</v>
       </c>
     </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2917,11 +2917,11 @@
       <c r="AP19" s="10"/>
       <c r="AQ19" s="10"/>
       <c r="AR19" s="4"/>
-      <c r="AS19" s="54">
+      <c r="AS19" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:45">
       <c r="A20" s="10">
         <v>18</v>
       </c>
@@ -2973,129 +2973,129 @@
       <c r="AP20" s="10"/>
       <c r="AQ20" s="10"/>
       <c r="AR20" s="4"/>
-      <c r="AS20" s="51">
+      <c r="AS20" s="50">
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A21" s="37">
+    <row r="21" spans="1:45">
+      <c r="A21" s="36">
         <v>19</v>
       </c>
-      <c r="B21" s="24">
+      <c r="B21" s="23">
         <v>7</v>
       </c>
-      <c r="C21" s="38">
-        <v>2</v>
-      </c>
-      <c r="D21" s="37">
+      <c r="C21" s="37">
+        <v>2</v>
+      </c>
+      <c r="D21" s="36">
         <v>0.2</v>
       </c>
-      <c r="E21" s="37">
-        <v>2</v>
-      </c>
-      <c r="F21" s="37">
+      <c r="E21" s="36">
+        <v>2</v>
+      </c>
+      <c r="F21" s="36">
         <v>0.1</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="38">
         <v>0.1</v>
       </c>
-      <c r="H21" s="38">
-        <v>2</v>
-      </c>
-      <c r="I21" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K21" s="37">
+      <c r="H21" s="37">
+        <v>2</v>
+      </c>
+      <c r="I21" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J21" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K21" s="36">
         <v>0.02</v>
       </c>
-      <c r="L21" s="39">
-        <v>1</v>
-      </c>
-      <c r="M21" s="38">
-        <v>1</v>
-      </c>
-      <c r="N21" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="O21" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="P21" s="37">
+      <c r="L21" s="38">
+        <v>1</v>
+      </c>
+      <c r="M21" s="37">
+        <v>1</v>
+      </c>
+      <c r="N21" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="O21" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P21" s="36">
         <v>0.6</v>
       </c>
-      <c r="Q21" s="39">
+      <c r="Q21" s="38">
         <v>0.6</v>
       </c>
-      <c r="R21" s="38">
-        <v>2</v>
-      </c>
-      <c r="S21" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="T21" s="37">
-        <v>1</v>
-      </c>
-      <c r="U21" s="37">
+      <c r="R21" s="37">
+        <v>2</v>
+      </c>
+      <c r="S21" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="T21" s="36">
+        <v>1</v>
+      </c>
+      <c r="U21" s="36">
         <v>0.2</v>
       </c>
-      <c r="V21" s="39">
-        <v>1</v>
-      </c>
-      <c r="W21" s="38">
-        <v>1</v>
-      </c>
-      <c r="X21" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="Y21" s="37">
-        <v>2</v>
-      </c>
-      <c r="Z21" s="37">
+      <c r="V21" s="38">
+        <v>1</v>
+      </c>
+      <c r="W21" s="37">
+        <v>1</v>
+      </c>
+      <c r="X21" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Y21" s="36">
+        <v>2</v>
+      </c>
+      <c r="Z21" s="36">
         <v>0.3</v>
       </c>
-      <c r="AA21" s="39">
-        <v>2</v>
-      </c>
-      <c r="AB21" s="38">
+      <c r="AA21" s="38">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="37">
         <v>0</v>
       </c>
-      <c r="AC21" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD21" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE21" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF21" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG21" s="38">
-        <v>1</v>
-      </c>
-      <c r="AH21" s="37">
-        <v>1</v>
-      </c>
-      <c r="AI21" s="37">
-        <v>1</v>
-      </c>
-      <c r="AJ21" s="37">
+      <c r="AC21" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD21" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE21" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF21" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG21" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="36">
+        <v>1</v>
+      </c>
+      <c r="AI21" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ21" s="36">
         <v>0.6</v>
       </c>
-      <c r="AK21" s="37">
-        <v>1</v>
-      </c>
-      <c r="AL21" s="38">
+      <c r="AK21" s="36">
+        <v>1</v>
+      </c>
+      <c r="AL21" s="37">
         <v>50</v>
       </c>
-      <c r="AM21" s="37">
+      <c r="AM21" s="36">
         <v>600</v>
       </c>
-      <c r="AN21" s="39">
+      <c r="AN21" s="38">
         <v>1200</v>
       </c>
       <c r="AO21" s="13" t="s">
@@ -3104,11 +3104,11 @@
       <c r="AP21" s="10"/>
       <c r="AQ21" s="10"/>
       <c r="AR21" s="4"/>
-      <c r="AS21" s="51">
+      <c r="AS21" s="50">
         <v>0.86111111111111116</v>
       </c>
     </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:45">
       <c r="A22" s="10">
         <v>20</v>
       </c>
@@ -3160,7 +3160,7 @@
       <c r="AP22" s="10"/>
       <c r="AQ22" s="10"/>
     </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:45">
       <c r="A23" s="10">
         <v>21</v>
       </c>
@@ -3213,135 +3213,135 @@
       <c r="AP23" s="10"/>
       <c r="AQ23" s="10"/>
     </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A24" s="46">
+    <row r="24" spans="1:45">
+      <c r="A24" s="45">
         <v>22</v>
       </c>
-      <c r="B24" s="46">
+      <c r="B24" s="45">
         <v>8</v>
       </c>
-      <c r="C24" s="47">
-        <v>1</v>
-      </c>
-      <c r="D24" s="48">
+      <c r="C24" s="46">
+        <v>1</v>
+      </c>
+      <c r="D24" s="47">
         <v>0.2</v>
       </c>
-      <c r="E24" s="48">
-        <v>1</v>
-      </c>
-      <c r="F24" s="48">
+      <c r="E24" s="47">
+        <v>1</v>
+      </c>
+      <c r="F24" s="47">
         <v>0.05</v>
       </c>
-      <c r="G24" s="49">
+      <c r="G24" s="48">
         <v>0.1</v>
       </c>
-      <c r="H24" s="47">
-        <v>2</v>
-      </c>
-      <c r="I24" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="J24" s="50" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" s="48">
+      <c r="H24" s="46">
+        <v>2</v>
+      </c>
+      <c r="I24" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="J24" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="K24" s="47">
         <v>0.02</v>
       </c>
-      <c r="L24" s="49">
+      <c r="L24" s="48">
         <v>0.15</v>
       </c>
-      <c r="M24" s="47">
-        <v>1</v>
-      </c>
-      <c r="N24" s="48">
+      <c r="M24" s="46">
+        <v>1</v>
+      </c>
+      <c r="N24" s="47">
         <v>0.6</v>
       </c>
-      <c r="O24" s="48">
-        <v>1</v>
-      </c>
-      <c r="P24" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="Q24" s="49">
-        <v>1</v>
-      </c>
-      <c r="R24" s="47">
-        <v>2</v>
-      </c>
-      <c r="S24" s="48">
-        <v>1</v>
-      </c>
-      <c r="T24" s="48">
-        <v>2</v>
-      </c>
-      <c r="U24" s="48">
+      <c r="O24" s="47">
+        <v>1</v>
+      </c>
+      <c r="P24" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="Q24" s="48">
+        <v>1</v>
+      </c>
+      <c r="R24" s="46">
+        <v>2</v>
+      </c>
+      <c r="S24" s="47">
+        <v>1</v>
+      </c>
+      <c r="T24" s="47">
+        <v>2</v>
+      </c>
+      <c r="U24" s="47">
         <v>0.4</v>
       </c>
-      <c r="V24" s="49">
-        <v>1</v>
-      </c>
-      <c r="W24" s="47">
-        <v>1</v>
-      </c>
-      <c r="X24" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="Y24" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z24" s="48">
+      <c r="V24" s="48">
+        <v>1</v>
+      </c>
+      <c r="W24" s="46">
+        <v>1</v>
+      </c>
+      <c r="X24" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="Y24" s="47">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="47">
         <v>0.3</v>
       </c>
-      <c r="AA24" s="49">
-        <v>2</v>
-      </c>
-      <c r="AB24" s="47">
-        <v>2</v>
-      </c>
-      <c r="AC24" s="48">
+      <c r="AA24" s="48">
+        <v>2</v>
+      </c>
+      <c r="AB24" s="46">
+        <v>2</v>
+      </c>
+      <c r="AC24" s="47">
         <v>0.6</v>
       </c>
-      <c r="AD24" s="48">
-        <v>1</v>
-      </c>
-      <c r="AE24" s="48">
+      <c r="AD24" s="47">
+        <v>1</v>
+      </c>
+      <c r="AE24" s="47">
         <v>0.2</v>
       </c>
-      <c r="AF24" s="49">
+      <c r="AF24" s="48">
         <v>0.25</v>
       </c>
-      <c r="AG24" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH24" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AI24" s="48">
-        <v>1</v>
-      </c>
-      <c r="AJ24" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AK24" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AL24" s="47">
+      <c r="AG24" s="46">
+        <v>1</v>
+      </c>
+      <c r="AH24" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AI24" s="47">
+        <v>1</v>
+      </c>
+      <c r="AJ24" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AK24" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AL24" s="46">
         <v>50</v>
       </c>
-      <c r="AM24" s="48">
+      <c r="AM24" s="47">
         <v>600</v>
       </c>
-      <c r="AN24" s="49">
+      <c r="AN24" s="48">
         <v>1200</v>
       </c>
       <c r="AO24" s="13"/>
       <c r="AP24" s="10"/>
       <c r="AQ24" s="10"/>
-      <c r="AS24" s="54">
+      <c r="AS24" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3392,11 +3392,11 @@
       <c r="AO25" s="13"/>
       <c r="AP25" s="10"/>
       <c r="AQ25" s="10"/>
-      <c r="AS25" s="54">
+      <c r="AS25" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -3447,139 +3447,139 @@
       <c r="AO26" s="13"/>
       <c r="AP26" s="10"/>
       <c r="AQ26" s="10"/>
-      <c r="AS26" s="54">
+      <c r="AS26" s="53">
         <v>0.83750000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A27" s="37">
+    <row r="27" spans="1:45">
+      <c r="A27" s="36">
         <v>25</v>
       </c>
-      <c r="B27" s="24">
+      <c r="B27" s="23">
         <v>9</v>
       </c>
-      <c r="C27" s="38">
-        <v>1</v>
-      </c>
-      <c r="D27" s="37">
+      <c r="C27" s="37">
+        <v>1</v>
+      </c>
+      <c r="D27" s="36">
         <v>0.1</v>
       </c>
-      <c r="E27" s="37">
-        <v>1</v>
-      </c>
-      <c r="F27" s="37">
+      <c r="E27" s="36">
+        <v>1</v>
+      </c>
+      <c r="F27" s="36">
         <v>0.1</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="38">
         <v>0.1</v>
       </c>
-      <c r="H27" s="38">
-        <v>2</v>
-      </c>
-      <c r="I27" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J27" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K27" s="37">
+      <c r="H27" s="37">
+        <v>2</v>
+      </c>
+      <c r="I27" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J27" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" s="36">
         <v>0.01</v>
       </c>
-      <c r="L27" s="39">
-        <v>1</v>
-      </c>
-      <c r="M27" s="38">
-        <v>1</v>
-      </c>
-      <c r="N27" s="37">
+      <c r="L27" s="38">
+        <v>1</v>
+      </c>
+      <c r="M27" s="37">
+        <v>1</v>
+      </c>
+      <c r="N27" s="36">
         <v>0.6</v>
       </c>
-      <c r="O27" s="37">
-        <v>1</v>
-      </c>
-      <c r="P27" s="37">
+      <c r="O27" s="36">
+        <v>1</v>
+      </c>
+      <c r="P27" s="36">
         <v>0.6</v>
       </c>
-      <c r="Q27" s="39">
-        <v>1</v>
-      </c>
-      <c r="R27" s="38">
-        <v>2</v>
-      </c>
-      <c r="S27" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="T27" s="37">
-        <v>2</v>
-      </c>
-      <c r="U27" s="37">
+      <c r="Q27" s="38">
+        <v>1</v>
+      </c>
+      <c r="R27" s="37">
+        <v>2</v>
+      </c>
+      <c r="S27" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="T27" s="36">
+        <v>2</v>
+      </c>
+      <c r="U27" s="36">
         <v>0.2</v>
       </c>
-      <c r="V27" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="W27" s="38">
-        <v>1</v>
-      </c>
-      <c r="X27" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="Y27" s="37">
-        <v>2</v>
-      </c>
-      <c r="Z27" s="37">
+      <c r="V27" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="W27" s="37">
+        <v>1</v>
+      </c>
+      <c r="X27" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Y27" s="36">
+        <v>2</v>
+      </c>
+      <c r="Z27" s="36">
         <v>0.4</v>
       </c>
-      <c r="AA27" s="39">
-        <v>2</v>
-      </c>
-      <c r="AB27" s="38">
-        <v>2</v>
-      </c>
-      <c r="AC27" s="37">
+      <c r="AA27" s="38">
+        <v>2</v>
+      </c>
+      <c r="AB27" s="37">
+        <v>2</v>
+      </c>
+      <c r="AC27" s="36">
         <v>0.6</v>
       </c>
-      <c r="AD27" s="37">
-        <v>1</v>
-      </c>
-      <c r="AE27" s="37">
+      <c r="AD27" s="36">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="36">
         <v>0.1</v>
       </c>
-      <c r="AF27" s="39">
-        <v>1</v>
-      </c>
-      <c r="AG27" s="38">
-        <v>1</v>
-      </c>
-      <c r="AH27" s="37">
-        <v>1</v>
-      </c>
-      <c r="AI27" s="37">
-        <v>2</v>
-      </c>
-      <c r="AJ27" s="37">
+      <c r="AF27" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH27" s="36">
+        <v>1</v>
+      </c>
+      <c r="AI27" s="36">
+        <v>2</v>
+      </c>
+      <c r="AJ27" s="36">
         <v>0.6</v>
       </c>
-      <c r="AK27" s="37">
-        <v>1</v>
-      </c>
-      <c r="AL27" s="38">
+      <c r="AK27" s="36">
+        <v>1</v>
+      </c>
+      <c r="AL27" s="37">
         <v>50</v>
       </c>
-      <c r="AM27" s="37">
+      <c r="AM27" s="36">
         <v>600</v>
       </c>
-      <c r="AN27" s="39">
+      <c r="AN27" s="38">
         <v>1200</v>
       </c>
       <c r="AO27" s="13"/>
       <c r="AP27" s="10"/>
       <c r="AQ27" s="10"/>
-      <c r="AS27" s="54">
+      <c r="AS27" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:45">
       <c r="A28" s="10">
         <v>26</v>
       </c>
@@ -3630,11 +3630,11 @@
       <c r="AO28" s="13"/>
       <c r="AP28" s="10"/>
       <c r="AQ28" s="10"/>
-      <c r="AS28" s="54">
+      <c r="AS28" s="53">
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:45">
       <c r="A29" s="10">
         <v>27</v>
       </c>
@@ -3685,129 +3685,129 @@
       <c r="AO29" s="13"/>
       <c r="AP29" s="10"/>
       <c r="AQ29" s="10"/>
-      <c r="AS29" s="54">
+      <c r="AS29" s="53">
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A30" s="48">
+    <row r="30" spans="1:45">
+      <c r="A30" s="47">
         <v>28</v>
       </c>
-      <c r="B30" s="46">
+      <c r="B30" s="45">
         <v>10</v>
       </c>
-      <c r="C30" s="47">
-        <v>2</v>
-      </c>
-      <c r="D30" s="48">
+      <c r="C30" s="46">
+        <v>2</v>
+      </c>
+      <c r="D30" s="47">
         <v>0.2</v>
       </c>
-      <c r="E30" s="48">
-        <v>1</v>
-      </c>
-      <c r="F30" s="48">
+      <c r="E30" s="47">
+        <v>1</v>
+      </c>
+      <c r="F30" s="47">
         <v>0.05</v>
       </c>
-      <c r="G30" s="49">
-        <v>1</v>
-      </c>
-      <c r="H30" s="47">
-        <v>1</v>
-      </c>
-      <c r="I30" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="J30" s="50" t="s">
-        <v>24</v>
-      </c>
-      <c r="K30" s="48">
+      <c r="G30" s="48">
+        <v>1</v>
+      </c>
+      <c r="H30" s="46">
+        <v>1</v>
+      </c>
+      <c r="I30" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" s="47">
         <v>0.02</v>
       </c>
-      <c r="L30" s="49">
-        <v>0.5</v>
-      </c>
-      <c r="M30" s="47">
-        <v>1</v>
-      </c>
-      <c r="N30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="O30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="P30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="Q30" s="49">
+      <c r="L30" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="M30" s="46">
+        <v>1</v>
+      </c>
+      <c r="N30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="O30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="P30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="Q30" s="48">
         <v>0.6</v>
       </c>
-      <c r="R30" s="47">
-        <v>1</v>
-      </c>
-      <c r="S30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="T30" s="48">
-        <v>1</v>
-      </c>
-      <c r="U30" s="48">
+      <c r="R30" s="46">
+        <v>1</v>
+      </c>
+      <c r="S30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="T30" s="47">
+        <v>1</v>
+      </c>
+      <c r="U30" s="47">
         <v>0.2</v>
       </c>
-      <c r="V30" s="49">
-        <v>0.5</v>
-      </c>
-      <c r="W30" s="47">
-        <v>1</v>
-      </c>
-      <c r="X30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="Y30" s="48">
-        <v>1</v>
-      </c>
-      <c r="Z30" s="48">
+      <c r="V30" s="48">
+        <v>0.5</v>
+      </c>
+      <c r="W30" s="46">
+        <v>1</v>
+      </c>
+      <c r="X30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="Y30" s="47">
+        <v>1</v>
+      </c>
+      <c r="Z30" s="47">
         <v>0.3</v>
       </c>
-      <c r="AA30" s="49">
-        <v>1</v>
-      </c>
-      <c r="AB30" s="47">
-        <v>1</v>
-      </c>
-      <c r="AC30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AD30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AE30" s="48">
+      <c r="AA30" s="48">
+        <v>1</v>
+      </c>
+      <c r="AB30" s="46">
+        <v>1</v>
+      </c>
+      <c r="AC30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AD30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AE30" s="47">
         <v>0.1</v>
       </c>
-      <c r="AF30" s="49">
+      <c r="AF30" s="48">
         <v>0.25</v>
       </c>
-      <c r="AG30" s="47">
-        <v>1</v>
-      </c>
-      <c r="AH30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AI30" s="48">
-        <v>1</v>
-      </c>
-      <c r="AJ30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AK30" s="48">
-        <v>0.5</v>
-      </c>
-      <c r="AL30" s="47">
+      <c r="AG30" s="46">
+        <v>1</v>
+      </c>
+      <c r="AH30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AI30" s="47">
+        <v>1</v>
+      </c>
+      <c r="AJ30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AK30" s="47">
+        <v>0.5</v>
+      </c>
+      <c r="AL30" s="46">
         <v>50</v>
       </c>
-      <c r="AM30" s="48">
+      <c r="AM30" s="47">
         <v>600</v>
       </c>
-      <c r="AN30" s="49">
+      <c r="AN30" s="48">
         <v>1200</v>
       </c>
       <c r="AO30" s="13" t="s">
@@ -3815,11 +3815,11 @@
       </c>
       <c r="AP30" s="10"/>
       <c r="AQ30" s="10"/>
-      <c r="AS30" s="54">
+      <c r="AS30" s="53">
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3872,11 +3872,11 @@
       </c>
       <c r="AP31" s="10"/>
       <c r="AQ31" s="10"/>
-      <c r="AS31" s="54">
+      <c r="AS31" s="53">
         <v>0.83680555555555547</v>
       </c>
     </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3929,139 +3929,139 @@
       </c>
       <c r="AP32" s="10"/>
       <c r="AQ32" s="10"/>
-      <c r="AS32" s="54">
+      <c r="AS32" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="33" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A33" s="24">
+    <row r="33" spans="1:45">
+      <c r="A33" s="23">
         <v>31</v>
       </c>
-      <c r="B33" s="24">
+      <c r="B33" s="23">
         <v>11</v>
       </c>
-      <c r="C33" s="38">
-        <v>2</v>
-      </c>
-      <c r="D33" s="37">
+      <c r="C33" s="37">
+        <v>2</v>
+      </c>
+      <c r="D33" s="36">
         <v>0.2</v>
       </c>
-      <c r="E33" s="37">
-        <v>2</v>
-      </c>
-      <c r="F33" s="37">
+      <c r="E33" s="36">
+        <v>2</v>
+      </c>
+      <c r="F33" s="36">
         <v>0.05</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="38">
         <v>0.1</v>
       </c>
-      <c r="H33" s="38">
-        <v>1</v>
-      </c>
-      <c r="I33" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J33" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K33" s="37">
+      <c r="H33" s="37">
+        <v>1</v>
+      </c>
+      <c r="I33" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J33" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" s="36">
         <v>0.02</v>
       </c>
-      <c r="L33" s="39">
+      <c r="L33" s="38">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M33" s="38">
-        <v>1</v>
-      </c>
-      <c r="N33" s="37">
+      <c r="M33" s="37">
+        <v>1</v>
+      </c>
+      <c r="N33" s="36">
         <v>0.6</v>
       </c>
-      <c r="O33" s="37">
-        <v>1</v>
-      </c>
-      <c r="P33" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="Q33" s="39">
-        <v>1</v>
-      </c>
-      <c r="R33" s="38">
-        <v>1</v>
-      </c>
-      <c r="S33" s="37">
-        <v>1</v>
-      </c>
-      <c r="T33" s="37">
-        <v>2</v>
-      </c>
-      <c r="U33" s="37">
+      <c r="O33" s="36">
+        <v>1</v>
+      </c>
+      <c r="P33" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Q33" s="38">
+        <v>1</v>
+      </c>
+      <c r="R33" s="37">
+        <v>1</v>
+      </c>
+      <c r="S33" s="36">
+        <v>1</v>
+      </c>
+      <c r="T33" s="36">
+        <v>2</v>
+      </c>
+      <c r="U33" s="36">
         <v>0.4</v>
       </c>
-      <c r="V33" s="39">
-        <v>1</v>
-      </c>
-      <c r="W33" s="38">
-        <v>1</v>
-      </c>
-      <c r="X33" s="37">
-        <v>1</v>
-      </c>
-      <c r="Y33" s="37">
-        <v>2</v>
-      </c>
-      <c r="Z33" s="37">
+      <c r="V33" s="38">
+        <v>1</v>
+      </c>
+      <c r="W33" s="37">
+        <v>1</v>
+      </c>
+      <c r="X33" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y33" s="36">
+        <v>2</v>
+      </c>
+      <c r="Z33" s="36">
         <v>0.4</v>
       </c>
-      <c r="AA33" s="39">
-        <v>1</v>
-      </c>
-      <c r="AB33" s="38">
+      <c r="AA33" s="38">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="37">
         <v>0</v>
       </c>
-      <c r="AC33" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD33" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE33" s="40" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF33" s="39" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG33" s="38">
-        <v>1</v>
-      </c>
-      <c r="AH33" s="37">
-        <v>1</v>
-      </c>
-      <c r="AI33" s="37">
-        <v>1</v>
-      </c>
-      <c r="AJ33" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AK33" s="37">
-        <v>1</v>
-      </c>
-      <c r="AL33" s="38">
+      <c r="AC33" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD33" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE33" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF33" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG33" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH33" s="36">
+        <v>1</v>
+      </c>
+      <c r="AI33" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ33" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AK33" s="36">
+        <v>1</v>
+      </c>
+      <c r="AL33" s="37">
         <v>50</v>
       </c>
-      <c r="AM33" s="37">
+      <c r="AM33" s="36">
         <v>600</v>
       </c>
-      <c r="AN33" s="39">
+      <c r="AN33" s="38">
         <v>1200</v>
       </c>
       <c r="AO33" s="13"/>
       <c r="AP33" s="10"/>
       <c r="AQ33" s="10"/>
-      <c r="AS33" s="54">
+      <c r="AS33" s="53">
         <v>0.83819444444444446</v>
       </c>
     </row>
-    <row r="34" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:45">
       <c r="A34" s="10">
         <v>32</v>
       </c>
@@ -4112,11 +4112,11 @@
       <c r="AO34" s="13"/>
       <c r="AP34" s="10"/>
       <c r="AQ34" s="10"/>
-      <c r="AS34" s="54">
+      <c r="AS34" s="53">
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="35" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:45">
       <c r="A35" s="10">
         <v>33</v>
       </c>
@@ -4167,139 +4167,139 @@
       <c r="AO35" s="13"/>
       <c r="AP35" s="10"/>
       <c r="AQ35" s="10"/>
-      <c r="AS35" s="54">
+      <c r="AS35" s="53">
         <v>0.89930555555555547</v>
       </c>
     </row>
-    <row r="36" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A36" s="45">
+    <row r="36" spans="1:45">
+      <c r="A36" s="44">
         <v>34</v>
       </c>
-      <c r="B36" s="41">
+      <c r="B36" s="40">
         <v>12</v>
       </c>
-      <c r="C36" s="42">
-        <v>2</v>
-      </c>
-      <c r="D36" s="45">
+      <c r="C36" s="41">
+        <v>2</v>
+      </c>
+      <c r="D36" s="44">
         <v>0.2</v>
       </c>
-      <c r="E36" s="45">
-        <v>2</v>
-      </c>
-      <c r="F36" s="45">
+      <c r="E36" s="44">
+        <v>2</v>
+      </c>
+      <c r="F36" s="44">
         <v>0.05</v>
       </c>
-      <c r="G36" s="44">
+      <c r="G36" s="43">
         <v>0.1</v>
       </c>
-      <c r="H36" s="42">
-        <v>1</v>
-      </c>
-      <c r="I36" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="J36" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="K36" s="45">
+      <c r="H36" s="41">
+        <v>1</v>
+      </c>
+      <c r="I36" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="K36" s="44">
         <v>0.02</v>
       </c>
-      <c r="L36" s="44">
-        <v>1</v>
-      </c>
-      <c r="M36" s="42">
-        <v>1</v>
-      </c>
-      <c r="N36" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="O36" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="P36" s="45">
+      <c r="L36" s="43">
+        <v>1</v>
+      </c>
+      <c r="M36" s="41">
+        <v>1</v>
+      </c>
+      <c r="N36" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="O36" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="P36" s="44">
         <v>0.6</v>
       </c>
-      <c r="Q36" s="44">
+      <c r="Q36" s="43">
         <v>0.6</v>
       </c>
-      <c r="R36" s="42">
-        <v>2</v>
-      </c>
-      <c r="S36" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="T36" s="45">
-        <v>1</v>
-      </c>
-      <c r="U36" s="45">
+      <c r="R36" s="41">
+        <v>2</v>
+      </c>
+      <c r="S36" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="T36" s="44">
+        <v>1</v>
+      </c>
+      <c r="U36" s="44">
         <v>0.4</v>
       </c>
-      <c r="V36" s="44">
-        <v>1</v>
-      </c>
-      <c r="W36" s="42">
-        <v>1</v>
-      </c>
-      <c r="X36" s="45">
-        <v>1</v>
-      </c>
-      <c r="Y36" s="45">
-        <v>1</v>
-      </c>
-      <c r="Z36" s="45">
+      <c r="V36" s="43">
+        <v>1</v>
+      </c>
+      <c r="W36" s="41">
+        <v>1</v>
+      </c>
+      <c r="X36" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y36" s="44">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="44">
         <v>0.4</v>
       </c>
-      <c r="AA36" s="44">
-        <v>1</v>
-      </c>
-      <c r="AB36" s="42">
+      <c r="AA36" s="43">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="41">
         <v>0</v>
       </c>
-      <c r="AC36" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD36" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE36" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF36" s="44" t="s">
-        <v>22</v>
-      </c>
-      <c r="AG36" s="42">
-        <v>1</v>
-      </c>
-      <c r="AH36" s="45">
-        <v>1</v>
-      </c>
-      <c r="AI36" s="45">
-        <v>1</v>
-      </c>
-      <c r="AJ36" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="AK36" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="AL36" s="42">
+      <c r="AC36" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD36" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="AE36" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF36" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG36" s="41">
+        <v>1</v>
+      </c>
+      <c r="AH36" s="44">
+        <v>1</v>
+      </c>
+      <c r="AI36" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ36" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="AK36" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="AL36" s="41">
         <v>50</v>
       </c>
-      <c r="AM36" s="45">
+      <c r="AM36" s="44">
         <v>600</v>
       </c>
-      <c r="AN36" s="44">
+      <c r="AN36" s="43">
         <v>1200</v>
       </c>
       <c r="AO36" s="13"/>
       <c r="AP36" s="10"/>
       <c r="AQ36" s="10"/>
-      <c r="AS36" s="54">
+      <c r="AS36" s="53">
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="37" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:45">
       <c r="A37" s="10">
         <v>35</v>
       </c>
@@ -4350,11 +4350,11 @@
       <c r="AO37" s="13"/>
       <c r="AP37" s="10"/>
       <c r="AQ37" s="10"/>
-      <c r="AS37" s="54">
+      <c r="AS37" s="53">
         <v>0.87152777777777779</v>
       </c>
     </row>
-    <row r="38" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4405,139 +4405,139 @@
       <c r="AO38" s="13"/>
       <c r="AP38" s="10"/>
       <c r="AQ38" s="10"/>
-      <c r="AS38" s="54">
+      <c r="AS38" s="53">
         <v>0.84305555555555556</v>
       </c>
     </row>
-    <row r="39" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A39" s="24">
+    <row r="39" spans="1:45">
+      <c r="A39" s="23">
         <v>37</v>
       </c>
-      <c r="B39" s="24">
+      <c r="B39" s="23">
         <v>13</v>
       </c>
-      <c r="C39" s="38">
-        <v>2</v>
-      </c>
-      <c r="D39" s="37">
+      <c r="C39" s="37">
+        <v>2</v>
+      </c>
+      <c r="D39" s="36">
         <v>0.1</v>
       </c>
-      <c r="E39" s="37">
-        <v>2</v>
-      </c>
-      <c r="F39" s="37">
+      <c r="E39" s="36">
+        <v>2</v>
+      </c>
+      <c r="F39" s="36">
         <v>0.1</v>
       </c>
-      <c r="G39" s="39">
+      <c r="G39" s="38">
         <v>0.1</v>
       </c>
-      <c r="H39" s="38">
-        <v>2</v>
-      </c>
-      <c r="I39" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J39" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K39" s="37">
+      <c r="H39" s="37">
+        <v>2</v>
+      </c>
+      <c r="I39" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J39" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K39" s="36">
         <v>0.02</v>
       </c>
-      <c r="L39" s="39">
-        <v>1</v>
-      </c>
-      <c r="M39" s="38">
-        <v>1</v>
-      </c>
-      <c r="N39" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="O39" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="P39" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="Q39" s="39">
+      <c r="L39" s="38">
+        <v>1</v>
+      </c>
+      <c r="M39" s="37">
+        <v>1</v>
+      </c>
+      <c r="N39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="O39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="Q39" s="38">
         <v>0.6</v>
       </c>
-      <c r="R39" s="38">
-        <v>1</v>
-      </c>
-      <c r="S39" s="37">
-        <v>1</v>
-      </c>
-      <c r="T39" s="37">
-        <v>2</v>
-      </c>
-      <c r="U39" s="37">
+      <c r="R39" s="37">
+        <v>1</v>
+      </c>
+      <c r="S39" s="36">
+        <v>1</v>
+      </c>
+      <c r="T39" s="36">
+        <v>2</v>
+      </c>
+      <c r="U39" s="36">
         <v>0.2</v>
       </c>
-      <c r="V39" s="39">
-        <v>0.5</v>
-      </c>
-      <c r="W39" s="38">
-        <v>1</v>
-      </c>
-      <c r="X39" s="37">
-        <v>1</v>
-      </c>
-      <c r="Y39" s="37">
-        <v>1</v>
-      </c>
-      <c r="Z39" s="37">
+      <c r="V39" s="38">
+        <v>0.5</v>
+      </c>
+      <c r="W39" s="37">
+        <v>1</v>
+      </c>
+      <c r="X39" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z39" s="36">
         <v>0.3</v>
       </c>
-      <c r="AA39" s="39">
-        <v>1</v>
-      </c>
-      <c r="AB39" s="38">
-        <v>2</v>
-      </c>
-      <c r="AC39" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AD39" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AE39" s="37">
+      <c r="AA39" s="38">
+        <v>1</v>
+      </c>
+      <c r="AB39" s="37">
+        <v>2</v>
+      </c>
+      <c r="AC39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AD39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AE39" s="36">
         <v>0.1</v>
       </c>
-      <c r="AF39" s="39">
-        <v>1</v>
-      </c>
-      <c r="AG39" s="38">
-        <v>1</v>
-      </c>
-      <c r="AH39" s="37">
-        <v>1</v>
-      </c>
-      <c r="AI39" s="37">
-        <v>1</v>
-      </c>
-      <c r="AJ39" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AK39" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AL39" s="38">
+      <c r="AF39" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH39" s="36">
+        <v>1</v>
+      </c>
+      <c r="AI39" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AK39" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AL39" s="37">
         <v>50</v>
       </c>
-      <c r="AM39" s="37">
+      <c r="AM39" s="36">
         <v>600</v>
       </c>
-      <c r="AN39" s="39">
+      <c r="AN39" s="38">
         <v>1200</v>
       </c>
       <c r="AO39" s="13"/>
       <c r="AP39" s="10"/>
       <c r="AQ39" s="10"/>
-      <c r="AS39" s="54">
+      <c r="AS39" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="40" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4588,11 +4588,11 @@
       <c r="AO40" s="13"/>
       <c r="AP40" s="10"/>
       <c r="AQ40" s="10"/>
-      <c r="AS40" s="54">
+      <c r="AS40" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="41" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:45">
       <c r="A41" s="10">
         <v>39</v>
       </c>
@@ -4643,139 +4643,139 @@
       <c r="AO41" s="13"/>
       <c r="AP41" s="10"/>
       <c r="AQ41" s="10"/>
-      <c r="AS41" s="54">
+      <c r="AS41" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="42" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A42" s="45">
+    <row r="42" spans="1:45">
+      <c r="A42" s="44">
         <v>40</v>
       </c>
-      <c r="B42" s="41">
+      <c r="B42" s="40">
         <v>14</v>
       </c>
-      <c r="C42" s="42">
-        <v>2</v>
-      </c>
-      <c r="D42" s="45">
+      <c r="C42" s="41">
+        <v>2</v>
+      </c>
+      <c r="D42" s="44">
         <v>0.2</v>
       </c>
-      <c r="E42" s="45">
-        <v>2</v>
-      </c>
-      <c r="F42" s="45">
+      <c r="E42" s="44">
+        <v>2</v>
+      </c>
+      <c r="F42" s="44">
         <v>0.1</v>
       </c>
-      <c r="G42" s="44">
+      <c r="G42" s="43">
         <v>0.1</v>
       </c>
-      <c r="H42" s="42">
-        <v>1</v>
-      </c>
-      <c r="I42" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="J42" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="K42" s="45">
+      <c r="H42" s="41">
+        <v>1</v>
+      </c>
+      <c r="I42" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="44">
         <v>0.02</v>
       </c>
-      <c r="L42" s="44">
+      <c r="L42" s="43">
         <v>0.15</v>
       </c>
-      <c r="M42" s="42">
-        <v>1</v>
-      </c>
-      <c r="N42" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="O42" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="P42" s="45">
+      <c r="M42" s="41">
+        <v>1</v>
+      </c>
+      <c r="N42" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="O42" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="P42" s="44">
         <v>0.6</v>
       </c>
-      <c r="Q42" s="44">
+      <c r="Q42" s="43">
         <v>0.6</v>
       </c>
-      <c r="R42" s="42">
-        <v>1</v>
-      </c>
-      <c r="S42" s="45">
-        <v>0.5</v>
-      </c>
-      <c r="T42" s="45">
-        <v>1</v>
-      </c>
-      <c r="U42" s="45">
+      <c r="R42" s="41">
+        <v>1</v>
+      </c>
+      <c r="S42" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="T42" s="44">
+        <v>1</v>
+      </c>
+      <c r="U42" s="44">
         <v>0.4</v>
       </c>
-      <c r="V42" s="44">
-        <v>1</v>
-      </c>
-      <c r="W42" s="42">
-        <v>1</v>
-      </c>
-      <c r="X42" s="45">
-        <v>1</v>
-      </c>
-      <c r="Y42" s="45">
-        <v>1</v>
-      </c>
-      <c r="Z42" s="45">
+      <c r="V42" s="43">
+        <v>1</v>
+      </c>
+      <c r="W42" s="41">
+        <v>1</v>
+      </c>
+      <c r="X42" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y42" s="44">
+        <v>1</v>
+      </c>
+      <c r="Z42" s="44">
         <v>0.4</v>
       </c>
-      <c r="AA42" s="44">
-        <v>2</v>
-      </c>
-      <c r="AB42" s="42">
-        <v>2</v>
-      </c>
-      <c r="AC42" s="45">
+      <c r="AA42" s="43">
+        <v>2</v>
+      </c>
+      <c r="AB42" s="41">
+        <v>2</v>
+      </c>
+      <c r="AC42" s="44">
         <v>0.6</v>
       </c>
-      <c r="AD42" s="45">
-        <v>1</v>
-      </c>
-      <c r="AE42" s="45">
+      <c r="AD42" s="44">
+        <v>1</v>
+      </c>
+      <c r="AE42" s="44">
         <v>0.1</v>
       </c>
-      <c r="AF42" s="44">
-        <v>1</v>
-      </c>
-      <c r="AG42" s="42">
-        <v>1</v>
-      </c>
-      <c r="AH42" s="45">
-        <v>1</v>
-      </c>
-      <c r="AI42" s="45">
-        <v>1</v>
-      </c>
-      <c r="AJ42" s="45">
+      <c r="AF42" s="43">
+        <v>1</v>
+      </c>
+      <c r="AG42" s="41">
+        <v>1</v>
+      </c>
+      <c r="AH42" s="44">
+        <v>1</v>
+      </c>
+      <c r="AI42" s="44">
+        <v>1</v>
+      </c>
+      <c r="AJ42" s="44">
         <v>0.6</v>
       </c>
-      <c r="AK42" s="45">
-        <v>1</v>
-      </c>
-      <c r="AL42" s="42">
+      <c r="AK42" s="44">
+        <v>1</v>
+      </c>
+      <c r="AL42" s="41">
         <v>50</v>
       </c>
-      <c r="AM42" s="45">
+      <c r="AM42" s="44">
         <v>600</v>
       </c>
-      <c r="AN42" s="44">
+      <c r="AN42" s="43">
         <v>1200</v>
       </c>
       <c r="AO42" s="13"/>
       <c r="AP42" s="10"/>
       <c r="AQ42" s="10"/>
-      <c r="AS42" s="54">
+      <c r="AS42" s="53">
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="43" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:45">
       <c r="A43" s="10">
         <v>41</v>
       </c>
@@ -4826,11 +4826,11 @@
       <c r="AO43" s="13"/>
       <c r="AP43" s="10"/>
       <c r="AQ43" s="10"/>
-      <c r="AS43" s="54">
+      <c r="AS43" s="53">
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="44" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:45">
       <c r="A44" s="10">
         <v>42</v>
       </c>
@@ -4882,132 +4882,132 @@
       <c r="AP44" s="10"/>
       <c r="AQ44" s="10"/>
     </row>
-    <row r="45" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="A45" s="24">
+    <row r="45" spans="1:45">
+      <c r="A45" s="23">
         <v>43</v>
       </c>
-      <c r="B45" s="24">
+      <c r="B45" s="23">
         <v>15</v>
       </c>
-      <c r="C45" s="38">
-        <v>2</v>
-      </c>
-      <c r="D45" s="37">
+      <c r="C45" s="37">
+        <v>2</v>
+      </c>
+      <c r="D45" s="36">
         <v>0.1</v>
       </c>
-      <c r="E45" s="37">
-        <v>2</v>
-      </c>
-      <c r="F45" s="37">
+      <c r="E45" s="36">
+        <v>2</v>
+      </c>
+      <c r="F45" s="36">
         <v>0.05</v>
       </c>
-      <c r="G45" s="39">
+      <c r="G45" s="38">
         <v>0.1</v>
       </c>
-      <c r="H45" s="38">
-        <v>1</v>
-      </c>
-      <c r="I45" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="J45" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="K45" s="37">
+      <c r="H45" s="37">
+        <v>1</v>
+      </c>
+      <c r="I45" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="J45" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45" s="36">
         <v>0.02</v>
       </c>
-      <c r="L45" s="39">
+      <c r="L45" s="38">
         <v>0.15</v>
       </c>
-      <c r="M45" s="38">
-        <v>1</v>
-      </c>
-      <c r="N45" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="O45" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="P45" s="37">
+      <c r="M45" s="37">
+        <v>1</v>
+      </c>
+      <c r="N45" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="O45" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="P45" s="36">
         <v>0.6</v>
       </c>
-      <c r="Q45" s="39">
+      <c r="Q45" s="38">
         <v>0.6</v>
       </c>
-      <c r="R45" s="38">
-        <v>1</v>
-      </c>
-      <c r="S45" s="37">
-        <v>1</v>
-      </c>
-      <c r="T45" s="37">
-        <v>2</v>
-      </c>
-      <c r="U45" s="37">
+      <c r="R45" s="37">
+        <v>1</v>
+      </c>
+      <c r="S45" s="36">
+        <v>1</v>
+      </c>
+      <c r="T45" s="36">
+        <v>2</v>
+      </c>
+      <c r="U45" s="36">
         <v>0.4</v>
       </c>
-      <c r="V45" s="39">
-        <v>1</v>
-      </c>
-      <c r="W45" s="38">
-        <v>1</v>
-      </c>
-      <c r="X45" s="37">
-        <v>1</v>
-      </c>
-      <c r="Y45" s="37">
-        <v>1</v>
-      </c>
-      <c r="Z45" s="37">
+      <c r="V45" s="38">
+        <v>1</v>
+      </c>
+      <c r="W45" s="37">
+        <v>1</v>
+      </c>
+      <c r="X45" s="36">
+        <v>1</v>
+      </c>
+      <c r="Y45" s="36">
+        <v>1</v>
+      </c>
+      <c r="Z45" s="36">
         <v>0.4</v>
       </c>
-      <c r="AA45" s="39">
-        <v>1</v>
-      </c>
-      <c r="AB45" s="38">
-        <v>2</v>
-      </c>
-      <c r="AC45" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AD45" s="37">
-        <v>0.5</v>
-      </c>
-      <c r="AE45" s="37">
+      <c r="AA45" s="38">
+        <v>1</v>
+      </c>
+      <c r="AB45" s="37">
+        <v>2</v>
+      </c>
+      <c r="AC45" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AD45" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="AE45" s="36">
         <v>0.2</v>
       </c>
-      <c r="AF45" s="39">
-        <v>1</v>
-      </c>
-      <c r="AG45" s="38">
-        <v>1</v>
-      </c>
-      <c r="AH45" s="37">
-        <v>1</v>
-      </c>
-      <c r="AI45" s="37">
-        <v>1</v>
-      </c>
-      <c r="AJ45" s="37">
+      <c r="AF45" s="38">
+        <v>1</v>
+      </c>
+      <c r="AG45" s="37">
+        <v>1</v>
+      </c>
+      <c r="AH45" s="36">
+        <v>1</v>
+      </c>
+      <c r="AI45" s="36">
+        <v>1</v>
+      </c>
+      <c r="AJ45" s="36">
         <v>0.6</v>
       </c>
-      <c r="AK45" s="37">
-        <v>1</v>
-      </c>
-      <c r="AL45" s="38">
+      <c r="AK45" s="36">
+        <v>1</v>
+      </c>
+      <c r="AL45" s="37">
         <v>50</v>
       </c>
-      <c r="AM45" s="37">
+      <c r="AM45" s="36">
         <v>600</v>
       </c>
-      <c r="AN45" s="39">
+      <c r="AN45" s="38">
         <v>1200</v>
       </c>
       <c r="AO45" s="13"/>
       <c r="AP45" s="10"/>
       <c r="AQ45" s="10"/>
     </row>
-    <row r="46" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -5059,55 +5059,55 @@
       <c r="AP46" s="10"/>
       <c r="AQ46" s="10"/>
     </row>
-    <row r="47" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="C47" s="17"/>
-      <c r="D47" s="18"/>
-      <c r="E47" s="18"/>
-      <c r="F47" s="18"/>
-      <c r="G47" s="19"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="18"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="18"/>
-      <c r="L47" s="19"/>
-      <c r="M47" s="17"/>
-      <c r="N47" s="18"/>
-      <c r="O47" s="18"/>
-      <c r="P47" s="18"/>
-      <c r="Q47" s="19"/>
-      <c r="R47" s="17"/>
-      <c r="S47" s="18"/>
-      <c r="T47" s="18"/>
-      <c r="U47" s="18"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="17"/>
-      <c r="X47" s="18"/>
-      <c r="Y47" s="18"/>
-      <c r="Z47" s="18"/>
-      <c r="AA47" s="19"/>
-      <c r="AB47" s="17"/>
-      <c r="AC47" s="18"/>
-      <c r="AD47" s="18"/>
-      <c r="AE47" s="18"/>
-      <c r="AF47" s="19"/>
-      <c r="AG47" s="17"/>
-      <c r="AH47" s="18"/>
-      <c r="AI47" s="18"/>
-      <c r="AJ47" s="18"/>
-      <c r="AK47" s="18"/>
-      <c r="AL47" s="17">
+      <c r="C47" s="16"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="17"/>
+      <c r="L47" s="18"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="18"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="18"/>
+      <c r="W47" s="16"/>
+      <c r="X47" s="17"/>
+      <c r="Y47" s="17"/>
+      <c r="Z47" s="17"/>
+      <c r="AA47" s="18"/>
+      <c r="AB47" s="16"/>
+      <c r="AC47" s="17"/>
+      <c r="AD47" s="17"/>
+      <c r="AE47" s="17"/>
+      <c r="AF47" s="18"/>
+      <c r="AG47" s="16"/>
+      <c r="AH47" s="17"/>
+      <c r="AI47" s="17"/>
+      <c r="AJ47" s="17"/>
+      <c r="AK47" s="17"/>
+      <c r="AL47" s="16">
         <v>150</v>
       </c>
-      <c r="AM47" s="18">
+      <c r="AM47" s="17">
         <v>600</v>
       </c>
-      <c r="AN47" s="21">
+      <c r="AN47" s="20">
         <v>1200</v>
       </c>
-      <c r="AO47" s="21"/>
+      <c r="AO47" s="20"/>
       <c r="AP47" s="10"/>
       <c r="AQ47" s="10"/>
     </row>

</xml_diff>